<commit_message>
changing template in excel
</commit_message>
<xml_diff>
--- a/InvoicePullData.xlsx
+++ b/InvoicePullData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8956c24d87df9e13/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saira\Desktop\DemoRobot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_E40E7D545B6E087E63072C165C059638C4F86BE4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{706A4642-6475-4229-8078-8ECB64F108FB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4428A7B8-039E-4FE4-A170-D4FECC0D35AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="77">
   <si>
     <t>Client Vendor No</t>
   </si>
@@ -245,6 +245,12 @@
   </si>
   <si>
     <t xml:space="preserve">4 RIVERS EQUIPMENT LLC                       </t>
+  </si>
+  <si>
+    <t>ShortDescription</t>
+  </si>
+  <si>
+    <t>Long Description</t>
   </si>
 </sst>
 </file>
@@ -297,10 +303,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -316,10 +323,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -619,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G653"/>
+  <dimension ref="A1:I653"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,7 +639,7 @@
     <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -658,8 +661,14 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -673,7 +682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -687,7 +696,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -701,7 +710,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -715,7 +724,7 @@
         <v>2308069</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -729,7 +738,7 @@
         <v>2308039</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -743,7 +752,7 @@
         <v>2308038</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -757,7 +766,7 @@
         <v>2308070</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -771,7 +780,7 @@
         <v>2308037</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -785,7 +794,7 @@
         <v>25400</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -799,7 +808,7 @@
         <v>25433</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -813,7 +822,7 @@
         <v>25434</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -827,7 +836,7 @@
         <v>25436</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -841,7 +850,7 @@
         <v>25437</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -855,7 +864,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>

</xml_diff>